<commit_message>
Implemeted extent report and logger
</commit_message>
<xml_diff>
--- a/src/test/resources/orangeHRMKeywords.xlsx
+++ b/src/test/resources/orangeHRMKeywords.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="58">
   <si>
     <t>TestCase ID</t>
   </si>
@@ -23,16 +23,16 @@
     <t>TestCase Name</t>
   </si>
   <si>
-    <t>Step Description</t>
-  </si>
-  <si>
-    <t>Locators</t>
-  </si>
-  <si>
-    <t>Action Keyword</t>
-  </si>
-  <si>
-    <t>Value</t>
+    <t>Test Step</t>
+  </si>
+  <si>
+    <t>Test Objects</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Test Data</t>
   </si>
   <si>
     <t>TC_01</t>
@@ -104,13 +104,40 @@
     <t>xpath=(//input[contains(@class,'oxd-input oxd-input--active')])[2]</t>
   </si>
   <si>
-    <t>Deepa</t>
+    <t>Peter.Anderson</t>
   </si>
   <si>
     <t>Click Search Button</t>
   </si>
   <si>
     <t>xpath=//button[contains(@class,'oxd-button oxd-button--medium oxd-button--secondary orangehrm-left-space')]</t>
+  </si>
+  <si>
+    <t>Validate Username in the result record</t>
+  </si>
+  <si>
+    <t>xpath=(//div[contains(@class,'oxd-table-cell oxd-padding-cell')]/div)[2]</t>
+  </si>
+  <si>
+    <t>validation</t>
+  </si>
+  <si>
+    <t>Click on User Profile</t>
+  </si>
+  <si>
+    <t>xpath=//p[contains(@class,'oxd-userdropdown-name')]</t>
+  </si>
+  <si>
+    <t>Click on Logout</t>
+  </si>
+  <si>
+    <t>xpath=(//a[contains(@class,'oxd-userdropdown-link')])[4]</t>
+  </si>
+  <si>
+    <t>Close the browser</t>
+  </si>
+  <si>
+    <t>closeBrowser</t>
   </si>
   <si>
     <t>TC_02</t>
@@ -169,12 +196,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -217,20 +244,52 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="Consolas"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -245,53 +304,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -307,6 +319,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
@@ -314,8 +341,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -330,7 +358,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -345,14 +373,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -367,31 +388,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -403,151 +562,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -561,22 +582,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -585,7 +601,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -605,17 +621,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -658,23 +668,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -684,131 +705,131 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -825,9 +846,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1149,10 +1167,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E12" sqref="$A1:$XFD1048576"/>
+      <selection activeCell="E18" sqref="$A1:$XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="5"/>
@@ -1288,15 +1306,74 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="3:5">
+    <row r="9" spans="3:6">
       <c r="C9" t="s">
         <v>30</v>
       </c>
       <c r="D9" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="5" t="s">
         <v>24</v>
+      </c>
+      <c r="F9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="3:6">
+      <c r="C10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="3:6">
+      <c r="C11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="3:6">
+      <c r="C12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="3:6">
+      <c r="C13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F13" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -1321,65 +1398,65 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="B1" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="C1" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="E1" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="F1" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="E2" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="5:6">
       <c r="E3" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="5:5">
       <c r="E4" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="5:6">
       <c r="E5" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="F5" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="5:6">
       <c r="E6" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>